<commit_message>
Evaluations results added, v4
</commit_message>
<xml_diff>
--- a/Evaluation/Tuning_Evaluation_Results.xlsx
+++ b/Evaluation/Tuning_Evaluation_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\UBC Research Period\Research\0_Latest Version\Data Chart Captioning System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\UBC Research Period\Research\0_Latest Version\Data Chart Captioning System\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD68A9F1-6D93-43CB-BA0B-0868681BA772}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65679E07-2C71-4F53-9DD8-9D442BEC5F75}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="6585" windowWidth="28290" windowHeight="2490" xr2:uid="{1019824F-6233-490B-85E9-0CFFF39F141C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{1019824F-6233-490B-85E9-0CFFF39F141C}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_M0" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="60">
   <si>
     <t>Sentence Generation</t>
   </si>
@@ -392,36 +392,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -432,12 +402,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,14 +416,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADCD9BA-5771-4F93-B998-D6E27EBA23CF}">
   <dimension ref="B2:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -789,42 +789,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="36" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="28" t="s">
+      <c r="M3" s="26"/>
+      <c r="N3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="37"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" s="3" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="4" t="s">
@@ -857,13 +857,13 @@
       <c r="K4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="18" t="s">
         <v>42</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="30" t="s">
+      <c r="N4" s="18" t="s">
         <v>42</v>
       </c>
       <c r="O4" s="10" t="s">
@@ -874,311 +874,345 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="19">
         <v>1E-3</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="19">
         <v>300</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="19">
         <v>64</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="19">
         <v>128</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="19">
         <v>128</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="19">
         <v>1E-3</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="19">
         <v>500</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="19">
         <v>64</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="19">
         <v>128</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="19">
         <v>128</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="19">
         <v>1E-3</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="19">
         <v>300</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="19">
         <v>64</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="19">
         <v>128</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="19">
         <v>128</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="33" t="s">
+      <c r="J7" s="19"/>
+      <c r="K7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="19">
         <v>1E-3</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="19">
         <v>200</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="19">
         <v>64</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="19">
         <v>128</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="19">
         <v>128</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="19">
         <v>770831</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
+      <c r="C9" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="F9" s="19">
+        <v>300</v>
+      </c>
+      <c r="G9" s="19">
+        <v>64</v>
+      </c>
+      <c r="H9" s="19">
+        <v>4</v>
+      </c>
+      <c r="I9" s="19">
+        <v>128</v>
+      </c>
+      <c r="J9" s="19">
+        <v>284231</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
+      <c r="C10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="F10" s="19">
+        <v>300</v>
+      </c>
+      <c r="G10" s="19">
+        <v>64</v>
+      </c>
+      <c r="H10" s="19">
+        <v>256</v>
+      </c>
+      <c r="I10" s="19">
+        <v>128</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="35" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="35"/>
-      <c r="K17" s="34" t="s">
+      <c r="J17" s="23"/>
+      <c r="K17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1206,19 +1240,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="36" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="28" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="37"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
@@ -1233,13 +1267,13 @@
       <c r="E5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I5" s="10" t="s">
@@ -1250,324 +1284,324 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="19">
         <v>2</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="19">
         <v>2</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="19">
         <v>2</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="19">
         <v>4</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="19">
         <v>2</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="19">
         <v>6</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="19">
         <v>4</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="19">
         <v>2</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="19">
         <v>4</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="19">
         <v>4</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="19">
         <v>4</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="19">
         <v>6</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="19">
         <v>6</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="19">
         <v>2</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="19">
         <v>6</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="19">
         <v>4</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="19">
         <v>8</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="19">
         <v>2</v>
       </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="19">
         <v>10</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="19">
         <v>2</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1593,60 +1627,60 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="16"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="17" t="s">
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="19"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="38"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="21" t="s">
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="21" t="s">
+      <c r="J8" s="31"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="22"/>
-      <c r="N8" s="23"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="32"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1" t="s">
@@ -1792,60 +1826,60 @@
       <c r="N15" s="13"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="16"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="35"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="19"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="38"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20" t="s">
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20" t="s">
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="21" t="s">
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M19" s="22"/>
-      <c r="N19" s="23"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="32"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="5" t="s">
@@ -1991,60 +2025,60 @@
       <c r="N26" s="13"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="16"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="35"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="17" t="s">
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="19"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="38"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20" t="s">
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20" t="s">
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="21" t="s">
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M30" s="22"/>
-      <c r="N30" s="23"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="32"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="1" t="s">
@@ -2204,60 +2238,60 @@
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="16"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="35"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="17" t="s">
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="19"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="38"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20" t="s">
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20" t="s">
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="21" t="s">
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M41" s="22"/>
-      <c r="N41" s="23"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="32"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="11" t="s">
@@ -2404,6 +2438,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C39:N39"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="I40:N40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="I30:K30"/>
@@ -2420,18 +2466,6 @@
     <mergeCell ref="C28:N28"/>
     <mergeCell ref="C29:H29"/>
     <mergeCell ref="I29:N29"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="C39:N39"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="I40:N40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L41:N41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add a stastistics dataframe
</commit_message>
<xml_diff>
--- a/Evaluation/Tuning_Evaluation_Results.xlsx
+++ b/Evaluation/Tuning_Evaluation_Results.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\UBC Research Period\Research\0_Latest Version\Data Chart Captioning System\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B738B-A516-42E2-B5FF-1E46615E1041}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E87E175-8692-4D88-8771-6A1C06612722}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="723" firstSheet="1" activeTab="4" xr2:uid="{1019824F-6233-490B-85E9-0CFFF39F141C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="723" firstSheet="1" activeTab="5" xr2:uid="{1019824F-6233-490B-85E9-0CFFF39F141C}"/>
   </bookViews>
   <sheets>
     <sheet name="All Tests" sheetId="5" r:id="rId1"/>
     <sheet name="Considered Tests" sheetId="8" r:id="rId2"/>
-    <sheet name="Test Categories" sheetId="7" r:id="rId3"/>
-    <sheet name="Test_M0_BS" sheetId="6" r:id="rId4"/>
-    <sheet name="Results" sheetId="4" r:id="rId5"/>
+    <sheet name="Foglio2" sheetId="10" r:id="rId3"/>
+    <sheet name="Test Categories" sheetId="7" r:id="rId4"/>
+    <sheet name="Test_M0_BS" sheetId="6" r:id="rId5"/>
+    <sheet name="Results" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="376">
   <si>
     <t>Sentence Generation</t>
   </si>
@@ -1154,6 +1155,15 @@
   </si>
   <si>
     <t>28.50</t>
+  </si>
+  <si>
+    <t>Config #</t>
+  </si>
+  <si>
+    <t>Opt</t>
+  </si>
+  <si>
+    <t>Embed</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1441,6 +1451,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1852,18 +1865,18 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="36" t="s">
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="39"/>
     </row>
     <row r="3" spans="2:19" s="2" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="17"/>
@@ -1875,22 +1888,22 @@
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39" t="s">
+      <c r="L3" s="40"/>
+      <c r="M3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39" t="s">
+      <c r="N3" s="40"/>
+      <c r="O3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39" t="s">
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="39"/>
+      <c r="R3" s="40"/>
     </row>
     <row r="4" spans="2:19" s="2" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="s">
@@ -2823,7 +2836,7 @@
   <dimension ref="A2:R12"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="Q12" sqref="A2:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2846,18 +2859,18 @@
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="36" t="s">
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="17"/>
@@ -2869,22 +2882,22 @@
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39" t="s">
+      <c r="M3" s="40"/>
+      <c r="N3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39" t="s">
+      <c r="O3" s="40"/>
+      <c r="P3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="39"/>
+      <c r="Q3" s="40"/>
     </row>
     <row r="4" spans="1:18" s="2" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="31" t="s">
@@ -3401,6 +3414,527 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69736115-77DC-4E93-9264-26C67EF40849}">
+  <dimension ref="B5:Q15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="B5:Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="39"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="40"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="F8" s="15">
+        <v>300</v>
+      </c>
+      <c r="G8" s="15">
+        <v>64</v>
+      </c>
+      <c r="H8" s="15">
+        <v>128</v>
+      </c>
+      <c r="I8" s="15">
+        <v>256</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q8" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="F9" s="15">
+        <v>300</v>
+      </c>
+      <c r="G9" s="15">
+        <v>64</v>
+      </c>
+      <c r="H9" s="15">
+        <v>256</v>
+      </c>
+      <c r="I9" s="15">
+        <v>256</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="F10" s="15">
+        <v>300</v>
+      </c>
+      <c r="G10" s="15">
+        <v>64</v>
+      </c>
+      <c r="H10" s="15">
+        <v>512</v>
+      </c>
+      <c r="I10" s="15">
+        <v>256</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F11" s="22">
+        <v>300</v>
+      </c>
+      <c r="G11" s="15">
+        <v>32</v>
+      </c>
+      <c r="H11" s="15">
+        <v>512</v>
+      </c>
+      <c r="I11" s="15">
+        <v>256</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="F12" s="15">
+        <v>300</v>
+      </c>
+      <c r="G12" s="15">
+        <v>128</v>
+      </c>
+      <c r="H12" s="15">
+        <v>512</v>
+      </c>
+      <c r="I12" s="15">
+        <v>256</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F13" s="22">
+        <v>300</v>
+      </c>
+      <c r="G13" s="15">
+        <v>32</v>
+      </c>
+      <c r="H13" s="15">
+        <v>512</v>
+      </c>
+      <c r="I13" s="15">
+        <v>512</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q13" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F14" s="22">
+        <v>300</v>
+      </c>
+      <c r="G14" s="15">
+        <v>32</v>
+      </c>
+      <c r="H14" s="15">
+        <v>512</v>
+      </c>
+      <c r="I14" s="15">
+        <v>128</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F15" s="22">
+        <v>300</v>
+      </c>
+      <c r="G15" s="15">
+        <v>32</v>
+      </c>
+      <c r="H15" s="15">
+        <v>512</v>
+      </c>
+      <c r="I15" s="15">
+        <v>64</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q15" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D458BE5-719F-453E-A172-B1B0F462FF91}">
   <dimension ref="B2:T15"/>
   <sheetViews>
@@ -3487,7 +4021,7 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="27" t="s">
@@ -3546,7 +4080,7 @@
       </c>
     </row>
     <row r="4" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="27" t="s">
         <v>27</v>
       </c>
@@ -3603,7 +4137,7 @@
       </c>
     </row>
     <row r="5" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="40"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="20">
         <v>3</v>
       </c>
@@ -3660,28 +4194,28 @@
       </c>
     </row>
     <row r="6" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="46"/>
     </row>
     <row r="7" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -3740,7 +4274,7 @@
       </c>
     </row>
     <row r="8" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="42"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="13" t="s">
         <v>29</v>
       </c>
@@ -3797,7 +4331,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="42"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="28" t="s">
         <v>31</v>
       </c>
@@ -3854,28 +4388,28 @@
       </c>
     </row>
     <row r="10" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="43"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="45"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="45"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="46"/>
     </row>
     <row r="11" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="29" t="s">
@@ -3932,7 +4466,7 @@
       <c r="T11" s="24"/>
     </row>
     <row r="12" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="47"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="29" t="s">
         <v>32</v>
       </c>
@@ -3987,7 +4521,7 @@
       <c r="T12" s="24"/>
     </row>
     <row r="13" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="47"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="12" t="s">
         <v>33</v>
       </c>
@@ -4042,7 +4576,7 @@
       <c r="T13" s="24"/>
     </row>
     <row r="14" spans="2:20" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="48"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="29" t="s">
         <v>34</v>
       </c>
@@ -4097,25 +4631,25 @@
       <c r="T14" s="23"/>
     </row>
     <row r="15" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="45"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4131,12 +4665,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7530DE53-98DE-4082-BEBC-44D0C75D831F}">
   <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:K7"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K17" sqref="B2:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4149,39 +4683,39 @@
     <row r="2" spans="2:12" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="36" t="s">
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="2:12" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39" t="s">
+      <c r="G3" s="40"/>
+      <c r="H3" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39" t="s">
+      <c r="I3" s="40"/>
+      <c r="J3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="39"/>
+      <c r="K3" s="40"/>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -4661,11 +5195,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098656CB-53FA-4AD4-BD2C-9B60511E8ECD}">
   <dimension ref="B6:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I31" sqref="I31:N35"/>
     </sheetView>
   </sheetViews>
@@ -4676,60 +5210,60 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="52"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="52" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="55"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="56" t="s">
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="57"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="56" t="s">
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="57"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="56" t="s">
+      <c r="J8" s="58"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="59"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1" t="s">
@@ -4979,60 +5513,60 @@
     </row>
     <row r="15" spans="2:14" ht="9" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="16" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="52"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="52" t="s">
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="55"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55" t="s">
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55" t="s">
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="56" t="s">
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="57"/>
-      <c r="N18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="59"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4" t="s">
@@ -5295,60 +5829,60 @@
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="52"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="52" t="s">
+      <c r="C28" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="52" t="s">
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="55"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55" t="s">
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55" t="s">
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="56" t="s">
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="M29" s="57"/>
-      <c r="N29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="59"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="9" t="s">
@@ -5598,6 +6132,20 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C27:N27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:N8"/>
     <mergeCell ref="C16:N16"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="I17:N17"/>
@@ -5605,20 +6153,6 @@
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="L18:N18"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="C27:N27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="I28:N28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="L29:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>